<commit_message>
output string by cached value
</commit_message>
<xml_diff>
--- a/data/sample1.xlsx
+++ b/data/sample1.xlsx
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -461,6 +461,16 @@
       </c>
       <c r="B3">
         <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <f>SUM(A2:A3)</f>
+        <v>56.7</v>
+      </c>
+      <c r="B4">
+        <f>AVERAGE(B2:B3)</f>
+        <v>79.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
time of excel formulas
</commit_message>
<xml_diff>
--- a/data/sample1.xlsx
+++ b/data/sample1.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="20" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="東京" sheetId="1" r:id="rId1"/>
     <sheet name="渋谷" sheetId="2" r:id="rId2"/>
+    <sheet name="新宿" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>気温</t>
     <rPh sb="0" eb="2">
@@ -74,11 +75,21 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>時刻</t>
+    <rPh sb="0" eb="2">
+      <t>ジコk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="h:mm;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -131,22 +142,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -545,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -612,4 +632,296 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.83203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>42978</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <f ca="1">A2+1</f>
+        <v>42979</v>
+      </c>
+      <c r="B3" s="5">
+        <f>B2+(1/24)</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <f ca="1">A3+1</f>
+        <v>42980</v>
+      </c>
+      <c r="B4" s="5">
+        <f t="shared" ref="B4:B23" si="0">B3+(1/24)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <f t="shared" ref="A5:A23" ca="1" si="1">A4+1</f>
+        <v>42981</v>
+      </c>
+      <c r="B5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42982</v>
+      </c>
+      <c r="B6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42983</v>
+      </c>
+      <c r="B7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.20833333333333331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42984</v>
+      </c>
+      <c r="B8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.24999999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42985</v>
+      </c>
+      <c r="B9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.29166666666666663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42986</v>
+      </c>
+      <c r="B10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42987</v>
+      </c>
+      <c r="B11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42988</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42989</v>
+      </c>
+      <c r="B13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45833333333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42990</v>
+      </c>
+      <c r="B14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42991</v>
+      </c>
+      <c r="B15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42992</v>
+      </c>
+      <c r="B16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42993</v>
+      </c>
+      <c r="B17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.62499999999999989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42994</v>
+      </c>
+      <c r="B18" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666652</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42995</v>
+      </c>
+      <c r="B19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.70833333333333315</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42996</v>
+      </c>
+      <c r="B20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.74999999999999978</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42997</v>
+      </c>
+      <c r="B21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.79166666666666641</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42998</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42999</v>
+      </c>
+      <c r="B23" s="5">
+        <f t="shared" si="0"/>
+        <v>0.87499999999999967</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <f t="shared" ref="A24:A27" ca="1" si="2">A23+1</f>
+        <v>43000</v>
+      </c>
+      <c r="B24" s="5">
+        <f t="shared" ref="B24:B27" si="3">B23+(1/24)</f>
+        <v>0.9166666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>43001</v>
+      </c>
+      <c r="B25" s="5">
+        <f t="shared" si="3"/>
+        <v>0.95833333333333293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>43002</v>
+      </c>
+      <c r="B26" s="5">
+        <f t="shared" si="3"/>
+        <v>0.99999999999999956</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>43003</v>
+      </c>
+      <c r="B27" s="5">
+        <f t="shared" si="3"/>
+        <v>1.0416666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
number and date format
</commit_message>
<xml_diff>
--- a/data/sample1.xlsx
+++ b/data/sample1.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="東京" sheetId="1" r:id="rId1"/>
     <sheet name="渋谷" sheetId="2" r:id="rId2"/>
     <sheet name="新宿" sheetId="3" r:id="rId3"/>
+    <sheet name="横浜" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>気温</t>
     <rPh sb="0" eb="2">
@@ -82,13 +83,23 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NAME</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="h:mm;@"/>
+  <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="h:mm;@"/>
+    <numFmt numFmtId="179" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="180" formatCode="yyyy/mm/dd\ h:mm"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -151,13 +162,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -638,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -658,7 +671,7 @@
     <row r="2" spans="1:2">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>42983</v>
+        <v>42989</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -667,7 +680,7 @@
     <row r="3" spans="1:2">
       <c r="A3" s="1">
         <f ca="1">A2+1</f>
-        <v>42984</v>
+        <v>42990</v>
       </c>
       <c r="B3" s="5">
         <f>B2+(1/24)</f>
@@ -677,7 +690,7 @@
     <row r="4" spans="1:2">
       <c r="A4" s="1">
         <f ca="1">A3+1</f>
-        <v>42985</v>
+        <v>42991</v>
       </c>
       <c r="B4" s="5">
         <f t="shared" ref="B4:B23" si="0">B3+(1/24)</f>
@@ -687,7 +700,7 @@
     <row r="5" spans="1:2">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A23" ca="1" si="1">A4+1</f>
-        <v>42986</v>
+        <v>42992</v>
       </c>
       <c r="B5" s="5">
         <f t="shared" si="0"/>
@@ -697,7 +710,7 @@
     <row r="6" spans="1:2">
       <c r="A6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42987</v>
+        <v>42993</v>
       </c>
       <c r="B6" s="5">
         <f t="shared" si="0"/>
@@ -707,7 +720,7 @@
     <row r="7" spans="1:2">
       <c r="A7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42988</v>
+        <v>42994</v>
       </c>
       <c r="B7" s="5">
         <f t="shared" si="0"/>
@@ -717,7 +730,7 @@
     <row r="8" spans="1:2">
       <c r="A8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42989</v>
+        <v>42995</v>
       </c>
       <c r="B8" s="5">
         <f t="shared" si="0"/>
@@ -727,7 +740,7 @@
     <row r="9" spans="1:2">
       <c r="A9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42990</v>
+        <v>42996</v>
       </c>
       <c r="B9" s="5">
         <f t="shared" si="0"/>
@@ -737,7 +750,7 @@
     <row r="10" spans="1:2">
       <c r="A10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42991</v>
+        <v>42997</v>
       </c>
       <c r="B10" s="5">
         <f t="shared" si="0"/>
@@ -747,7 +760,7 @@
     <row r="11" spans="1:2">
       <c r="A11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42992</v>
+        <v>42998</v>
       </c>
       <c r="B11" s="5">
         <f t="shared" si="0"/>
@@ -757,7 +770,7 @@
     <row r="12" spans="1:2">
       <c r="A12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42993</v>
+        <v>42999</v>
       </c>
       <c r="B12" s="5">
         <f t="shared" si="0"/>
@@ -767,7 +780,7 @@
     <row r="13" spans="1:2">
       <c r="A13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42994</v>
+        <v>43000</v>
       </c>
       <c r="B13" s="5">
         <f t="shared" si="0"/>
@@ -777,7 +790,7 @@
     <row r="14" spans="1:2">
       <c r="A14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42995</v>
+        <v>43001</v>
       </c>
       <c r="B14" s="5">
         <f t="shared" si="0"/>
@@ -787,7 +800,7 @@
     <row r="15" spans="1:2">
       <c r="A15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42996</v>
+        <v>43002</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" si="0"/>
@@ -797,7 +810,7 @@
     <row r="16" spans="1:2">
       <c r="A16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42997</v>
+        <v>43003</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" si="0"/>
@@ -807,7 +820,7 @@
     <row r="17" spans="1:2">
       <c r="A17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42998</v>
+        <v>43004</v>
       </c>
       <c r="B17" s="5">
         <f t="shared" si="0"/>
@@ -817,7 +830,7 @@
     <row r="18" spans="1:2">
       <c r="A18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42999</v>
+        <v>43005</v>
       </c>
       <c r="B18" s="5">
         <f t="shared" si="0"/>
@@ -827,7 +840,7 @@
     <row r="19" spans="1:2">
       <c r="A19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43000</v>
+        <v>43006</v>
       </c>
       <c r="B19" s="5">
         <f t="shared" si="0"/>
@@ -837,7 +850,7 @@
     <row r="20" spans="1:2">
       <c r="A20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43001</v>
+        <v>43007</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" si="0"/>
@@ -847,7 +860,7 @@
     <row r="21" spans="1:2">
       <c r="A21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43002</v>
+        <v>43008</v>
       </c>
       <c r="B21" s="5">
         <f t="shared" si="0"/>
@@ -857,7 +870,7 @@
     <row r="22" spans="1:2">
       <c r="A22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43003</v>
+        <v>43009</v>
       </c>
       <c r="B22" s="5">
         <f t="shared" si="0"/>
@@ -867,7 +880,7 @@
     <row r="23" spans="1:2">
       <c r="A23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43004</v>
+        <v>43010</v>
       </c>
       <c r="B23" s="5">
         <f t="shared" si="0"/>
@@ -877,7 +890,7 @@
     <row r="24" spans="1:2">
       <c r="A24" s="1">
         <f t="shared" ref="A24:A28" ca="1" si="2">A23+1</f>
-        <v>43005</v>
+        <v>43011</v>
       </c>
       <c r="B24" s="5">
         <f t="shared" ref="B24:B28" si="3">B23+(1/24)</f>
@@ -887,7 +900,7 @@
     <row r="25" spans="1:2">
       <c r="A25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43006</v>
+        <v>43012</v>
       </c>
       <c r="B25" s="5">
         <f t="shared" si="3"/>
@@ -897,7 +910,7 @@
     <row r="26" spans="1:2">
       <c r="A26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43007</v>
+        <v>43013</v>
       </c>
       <c r="B26" s="5">
         <f t="shared" si="3"/>
@@ -907,7 +920,7 @@
     <row r="27" spans="1:2">
       <c r="A27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43008</v>
+        <v>43014</v>
       </c>
       <c r="B27" s="5">
         <f t="shared" si="3"/>
@@ -917,7 +930,7 @@
     <row r="28" spans="1:2">
       <c r="A28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43009</v>
+        <v>43015</v>
       </c>
       <c r="B28" s="5">
         <f t="shared" si="3"/>
@@ -934,4 +947,69 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>123456789</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42758.46597222222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1234567890</v>
+      </c>
+      <c r="B3" s="6">
+        <v>42758.46597222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>12345678901</v>
+      </c>
+      <c r="B4" s="7">
+        <v>42758.46597222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>123456789012</v>
+      </c>
+      <c r="B5" s="5">
+        <v>42758.46597222222</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
not use mutli byte char
</commit_message>
<xml_diff>
--- a/data/sample1.xlsx
+++ b/data/sample1.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tak/Documents/git/Excel-Extraction/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E618F1BF-C330-F449-BBF5-2AE12987F3FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="東京" sheetId="1" r:id="rId1"/>
     <sheet name="渋谷" sheetId="2" r:id="rId2"/>
     <sheet name="新宿" sheetId="3" r:id="rId3"/>
     <sheet name="横浜" sheetId="4" r:id="rId4"/>
+    <sheet name="Tokyo" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>気温</t>
     <rPh sb="0" eb="2">
@@ -95,30 +102,38 @@
     <t>NUM</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="h:mm;@"/>
-    <numFmt numFmtId="179" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="180" formatCode="yyyy/mm/dd\ h:mm"/>
-    <numFmt numFmtId="181" formatCode="0.0_ "/>
-    <numFmt numFmtId="182" formatCode="0.00_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="0.0_ "/>
+    <numFmt numFmtId="167" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -127,7 +142,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -136,7 +151,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -176,25 +191,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -519,16 +542,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -539,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42736</v>
       </c>
@@ -550,7 +573,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43019</v>
       </c>
@@ -561,7 +584,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -587,19 +610,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -610,7 +633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>43040.003472222219</v>
       </c>
@@ -618,7 +641,7 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>43040.006944444445</v>
       </c>
@@ -629,7 +652,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>43040.010416666664</v>
       </c>
@@ -637,7 +660,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>43040.013888888891</v>
       </c>
@@ -660,19 +683,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -680,269 +703,269 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>42990</v>
+        <v>43552</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f ca="1">A2+1</f>
-        <v>42991</v>
+        <v>43553</v>
       </c>
       <c r="B3" s="5">
         <f>B2+(1/24)</f>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f ca="1">A3+1</f>
-        <v>42992</v>
+        <v>43554</v>
       </c>
       <c r="B4" s="5">
         <f t="shared" ref="B4:B23" si="0">B3+(1/24)</f>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A23" ca="1" si="1">A4+1</f>
-        <v>42993</v>
+        <v>43555</v>
       </c>
       <c r="B5" s="5">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42994</v>
+        <v>43556</v>
       </c>
       <c r="B6" s="5">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42995</v>
+        <v>43557</v>
       </c>
       <c r="B7" s="5">
         <f t="shared" si="0"/>
         <v>0.20833333333333331</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42996</v>
+        <v>43558</v>
       </c>
       <c r="B8" s="5">
         <f t="shared" si="0"/>
         <v>0.24999999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42997</v>
+        <v>43559</v>
       </c>
       <c r="B9" s="5">
         <f t="shared" si="0"/>
         <v>0.29166666666666663</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42998</v>
+        <v>43560</v>
       </c>
       <c r="B10" s="5">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42999</v>
+        <v>43561</v>
       </c>
       <c r="B11" s="5">
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43000</v>
+        <v>43562</v>
       </c>
       <c r="B12" s="5">
         <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43001</v>
+        <v>43563</v>
       </c>
       <c r="B13" s="5">
         <f t="shared" si="0"/>
         <v>0.45833333333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43002</v>
+        <v>43564</v>
       </c>
       <c r="B14" s="5">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43003</v>
+        <v>43565</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" si="0"/>
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43004</v>
+        <v>43566</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" si="0"/>
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43005</v>
+        <v>43567</v>
       </c>
       <c r="B17" s="5">
         <f t="shared" si="0"/>
         <v>0.62499999999999989</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43006</v>
+        <v>43568</v>
       </c>
       <c r="B18" s="5">
         <f t="shared" si="0"/>
         <v>0.66666666666666652</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43007</v>
+        <v>43569</v>
       </c>
       <c r="B19" s="5">
         <f t="shared" si="0"/>
         <v>0.70833333333333315</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43008</v>
+        <v>43570</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" si="0"/>
         <v>0.74999999999999978</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43009</v>
+        <v>43571</v>
       </c>
       <c r="B21" s="5">
         <f t="shared" si="0"/>
         <v>0.79166666666666641</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43010</v>
+        <v>43572</v>
       </c>
       <c r="B22" s="5">
         <f t="shared" si="0"/>
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43011</v>
+        <v>43573</v>
       </c>
       <c r="B23" s="5">
         <f t="shared" si="0"/>
         <v>0.87499999999999967</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <f t="shared" ref="A24:A28" ca="1" si="2">A23+1</f>
-        <v>43012</v>
+        <v>43574</v>
       </c>
       <c r="B24" s="5">
         <f t="shared" ref="B24:B28" si="3">B23+(1/24)</f>
         <v>0.9166666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43013</v>
+        <v>43575</v>
       </c>
       <c r="B25" s="5">
         <f t="shared" si="3"/>
         <v>0.95833333333333293</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43014</v>
+        <v>43576</v>
       </c>
       <c r="B26" s="5">
         <f t="shared" si="3"/>
         <v>0.99999999999999956</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43015</v>
+        <v>43577</v>
       </c>
       <c r="B27" s="5">
         <f t="shared" si="3"/>
         <v>1.0416666666666663</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43016</v>
+        <v>43578</v>
       </c>
       <c r="B28" s="5">
         <f t="shared" si="3"/>
@@ -962,20 +985,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -986,7 +1009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123456789</v>
       </c>
@@ -997,7 +1020,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1234567890</v>
       </c>
@@ -1008,7 +1031,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>12345678901</v>
       </c>
@@ -1019,7 +1042,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>123456789012</v>
       </c>
@@ -1040,4 +1063,63 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3227E1-DA6B-4F4E-A1EC-DE009203A719}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>1.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>